<commit_message>
German FCL templates updated
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_de.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_de.xlsx
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>MHD oder Verbrauchsdatum</t>
-  </si>
-  <si>
-    <t>Digitale Auszüge (z.B. Excel oder xml-Dateien) vom befragten Betrieb könnten ebenso geeignet sein; das Ausfüllen dieser Vorlage wäre dann nicht notwendig - für diesen Fall bitte Rückruf (Dr. Armin Weiser: 030 - 18412-2118)</t>
   </si>
   <si>
     <t>Die Warenausgänge sind bekannt (siehe oben, graue Felder)</t>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Bei Rückfragen bitte einfach Kontakt aufnehmen mit dem BfR FoodRiskLabs-Team, +49 (30) 18412-4444, foodrisklabs@bfr.bund.de</t>
+  </si>
+  <si>
+    <t>Digitale Auszüge (z.B. Excel oder xml-Dateien) vom befragten Betrieb könnten ebenso geeignet sein; das Ausfüllen dieser Vorlage wäre dann nicht notwendig - für diesen Fall bitte Rückruf (BfR FoodRiskLabs-Team, +49 (30) 18412-4444)</t>
   </si>
 </sst>
 </file>
@@ -1880,7 +1880,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="33" customFormat="1" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="71" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="72"/>
       <c r="C1" s="73"/>
@@ -1902,7 +1902,7 @@
     </row>
     <row r="2" spans="1:18" s="36" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -1941,24 +1941,24 @@
     </row>
     <row r="4" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="55"/>
       <c r="H4" s="55"/>
       <c r="I4" s="52"/>
       <c r="J4" s="47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="48"/>
@@ -1970,7 +1970,7 @@
     <row r="5" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40"/>
       <c r="B5" s="47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>5</v>
@@ -1982,21 +1982,21 @@
         <v>7</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="48"/>
       <c r="I5" s="64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="66" t="s">
-        <v>14</v>
-      </c>
       <c r="L5" s="66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" s="45"/>
       <c r="N5" s="9"/>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="7" spans="1:18" s="8" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="8" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="9" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="10" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="11" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="12" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="13" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="14" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="15" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="62"/>
       <c r="C15" s="62"/>
@@ -2164,24 +2164,24 @@
     </row>
     <row r="16" spans="1:18" s="17" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="52"/>
       <c r="D16" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="52"/>
       <c r="F16" s="68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="70"/>
       <c r="H16" s="70"/>
       <c r="I16" s="52"/>
       <c r="J16" s="49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="50"/>
       <c r="L16" s="48"/>
@@ -2192,7 +2192,7 @@
     <row r="17" spans="1:13" s="17" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="40"/>
       <c r="B17" s="57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="57" t="s">
         <v>5</v>
@@ -2204,21 +2204,21 @@
         <v>7</v>
       </c>
       <c r="F17" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="69"/>
       <c r="H17" s="52"/>
       <c r="I17" s="57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J17" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="67" t="s">
-        <v>14</v>
-      </c>
       <c r="L17" s="67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="38"/>
     </row>

</xml_diff>